<commit_message>
Update Exercise in calculating Information Gain in Decision Trees.xlsx
</commit_message>
<xml_diff>
--- a/4.Decision Tree - Calculating Information Gain/Exercise in calculating Information Gain in Decision Trees.xlsx
+++ b/4.Decision Tree - Calculating Information Gain/Exercise in calculating Information Gain in Decision Trees.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\9.Docencia\1.MATERIAS\2.IA y ML\2.PRÁCTICAS\Práctica9. ExplicacionPredicciones RF_RN_CNN_SVM\Extras - Ejercicios - Práctica de Modelo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhurtadoo\Proyectos\Data-Science-AI-Portfolio-Experiments-Predictions-and-Analysis\4.Decision Tree - Calculating Information Gain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EC4391-411B-4DA7-B9B8-6A43BF5E75F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00DA954-8A32-4F78-A54D-0085274051B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="660" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -170,13 +170,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>704034</xdr:colOff>
+      <xdr:colOff>707844</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>3061</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7893699" cy="526811"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="8036624" cy="526811"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -190,8 +190,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="704034" y="3067448"/>
-              <a:ext cx="7893699" cy="526811"/>
+              <a:off x="707844" y="3137093"/>
+              <a:ext cx="8036624" cy="526811"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -228,7 +228,19 @@
                     <a:rPr lang="en-US" sz="2000" b="0" i="1">
                       <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                     </a:rPr>
-                    <m:t>𝑛𝑓𝑜𝑟𝑚𝑡𝑖𝑜𝑛</m:t>
+                    <m:t>𝑛𝑓𝑜𝑟𝑚</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="es-EC" sz="2000" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>𝑎</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="2000" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>𝑡𝑖𝑜𝑛</m:t>
                   </m:r>
                   <m:r>
                     <a:rPr lang="en-US" sz="2000" b="0" i="1">
@@ -580,7 +592,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -594,8 +606,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="704034" y="3067448"/>
-              <a:ext cx="7893699" cy="526811"/>
+              <a:off x="707844" y="3137093"/>
+              <a:ext cx="8036624" cy="526811"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -630,7 +642,19 @@
                 <a:rPr lang="en-US" sz="2000" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑛𝑓𝑜𝑟𝑚𝑡𝑖𝑜𝑛 𝐺𝑎𝑖𝑛→ 𝐼𝐺(𝐷_𝑝,𝑓)=𝐼(𝐷_𝑃 )−𝑁_𝑙𝑒𝑓𝑡/𝑁_𝑝  𝐼(𝐷_𝑙𝑒𝑓𝑡 )−𝑁_𝑟𝑖𝑔ℎ𝑡/𝑁_𝑝  𝐼(𝐷_𝑟𝑖𝑔ℎ𝑡)</a:t>
+                <a:t>𝑛𝑓𝑜𝑟𝑚</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-EC" sz="2000" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑎</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="2000" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑡𝑖𝑜𝑛 𝐺𝑎𝑖𝑛→ 𝐼𝐺(𝐷_𝑝,𝑓)=𝐼(𝐷_𝑃 )−𝑁_𝑙𝑒𝑓𝑡/𝑁_𝑝  𝐼(𝐷_𝑙𝑒𝑓𝑡 )−𝑁_𝑟𝑖𝑔ℎ𝑡/𝑁_𝑝  𝐼(𝐷_𝑟𝑖𝑔ℎ𝑡)</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="2000"/>
             </a:p>
@@ -1451,13 +1475,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>704034</xdr:colOff>
+      <xdr:colOff>707844</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>3061</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7893699" cy="526811"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="8036624" cy="526811"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -1471,8 +1495,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="704034" y="3112021"/>
-              <a:ext cx="7893699" cy="526811"/>
+              <a:off x="707844" y="3137093"/>
+              <a:ext cx="8036624" cy="526811"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1509,7 +1533,19 @@
                     <a:rPr lang="en-US" sz="2000" b="0" i="1">
                       <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                     </a:rPr>
-                    <m:t>𝑛𝑓𝑜𝑟𝑚𝑡𝑖𝑜𝑛</m:t>
+                    <m:t>𝑛𝑓𝑜𝑟𝑚</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="es-EC" sz="2000" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>𝑎</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="2000" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>𝑡𝑖𝑜𝑛</m:t>
                   </m:r>
                   <m:r>
                     <a:rPr lang="en-US" sz="2000" b="0" i="1">
@@ -1861,7 +1897,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -1875,8 +1911,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="704034" y="3112021"/>
-              <a:ext cx="7893699" cy="526811"/>
+              <a:off x="707844" y="3137093"/>
+              <a:ext cx="8036624" cy="526811"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1911,7 +1947,19 @@
                 <a:rPr lang="en-US" sz="2000" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑛𝑓𝑜𝑟𝑚𝑡𝑖𝑜𝑛 𝐺𝑎𝑖𝑛→ 𝐼𝐺(𝐷_𝑝,𝑓)=𝐼(𝐷_𝑃 )−𝑁_𝑙𝑒𝑓𝑡/𝑁_𝑝  𝐼(𝐷_𝑙𝑒𝑓𝑡 )−𝑁_𝑟𝑖𝑔ℎ𝑡/𝑁_𝑝  𝐼(𝐷_𝑟𝑖𝑔ℎ𝑡)</a:t>
+                <a:t>𝑛𝑓𝑜𝑟𝑚</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-EC" sz="2000" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑎</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="2000" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑡𝑖𝑜𝑛 𝐺𝑎𝑖𝑛→ 𝐼𝐺(𝐷_𝑝,𝑓)=𝐼(𝐷_𝑃 )−𝑁_𝑙𝑒𝑓𝑡/𝑁_𝑝  𝐼(𝐷_𝑙𝑒𝑓𝑡 )−𝑁_𝑟𝑖𝑔ℎ𝑡/𝑁_𝑝  𝐼(𝐷_𝑟𝑖𝑔ℎ𝑡)</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="2000"/>
             </a:p>
@@ -3029,7 +3077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H15"/>
   <sheetViews>
-    <sheetView zoomScale="93" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="93" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -3201,8 +3249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB4335B-1FB9-46FF-BD76-3538AC2B1BE7}">
   <dimension ref="B2:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="93" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>